<commit_message>
[Document, Modified]: TaskList Specification & Login-Logout Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Use-case/Login_Logout/Login_Logout Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Use-case/Login_Logout/Login_Logout Specification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Logout" sheetId="1" state="visible" r:id="rId2"/>
@@ -475,11 +475,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,7 +538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -632,15 +632,15 @@
   </sheetPr>
   <dimension ref="B3:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -806,11 +806,11 @@
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -914,7 +914,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>58</v>
@@ -1012,11 +1012,11 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1075,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1178,15 +1178,15 @@
   </sheetPr>
   <dimension ref="B3:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1348,15 +1348,15 @@
   </sheetPr>
   <dimension ref="B3:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,7 +1424,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="97" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>75</v>
@@ -1518,15 +1518,15 @@
   </sheetPr>
   <dimension ref="B3:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,7 +1603,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>94</v>

</xml_diff>